<commit_message>
Update Regresi Tanggal 31/03/2023
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKAKT062-001 - Setup Periode Harian  - Tambah Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKAKT062-001 - Setup Periode Harian  - Tambah Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DPLK 2\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCADB01C-3490-4FD9-BACF-73FAD69850D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DDA06F-75A3-42E2-BE09-7F72B9A0C1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3645" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPLKAKT062-001" sheetId="2" r:id="rId1"/>
@@ -123,10 +123,10 @@
     <t>750</t>
   </si>
   <si>
-    <t>05/05/2023</t>
-  </si>
-  <si>
     <t>PERIODE_HARIAN</t>
+  </si>
+  <si>
+    <t>07/09/2024</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -625,7 +625,7 @@
         <v>20</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>21</v>
@@ -685,11 +685,11 @@
         <v>30</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P2" s="10" t="str">
         <f>RIGHT(O2,4) &amp; MID(O2,4,2) &amp; LEFT(O2,2)</f>
-        <v>20230505</v>
+        <v>20240907</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>24</v>

</xml_diff>